<commit_message>
added circuito final y dise~no
</commit_message>
<xml_diff>
--- a/Diseño/seleccion_componentes_sk_conf4.xlsx
+++ b/Diseño/seleccion_componentes_sk_conf4.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaco\Desktop\repos\TC\TP7\Diseño\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\ITBA\3er año\1er cuatri\TC\TP7\TP7NO\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053BEE54-8C94-4903-957A-8134B6FBCE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC97668-2BFD-46B0-99A6-15C26196B1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="2316" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{721602D0-5018-4882-9828-FB7C87249B7E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{721602D0-5018-4882-9828-FB7C87249B7E}"/>
   </bookViews>
   <sheets>
-    <sheet name="STAGE 5" sheetId="1" r:id="rId1"/>
-    <sheet name="STAGE 4" sheetId="2" r:id="rId2"/>
-    <sheet name="STAGE 3" sheetId="4" r:id="rId3"/>
-    <sheet name="STAGE 2" sheetId="5" r:id="rId4"/>
+    <sheet name="STAGE6" sheetId="7" r:id="rId1"/>
+    <sheet name="STAGE 5" sheetId="1" r:id="rId2"/>
+    <sheet name="STAGE 4" sheetId="2" r:id="rId3"/>
+    <sheet name="STAGE 3" sheetId="4" r:id="rId4"/>
+    <sheet name="STAGE 2" sheetId="5" r:id="rId5"/>
+    <sheet name="STAGE1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="35">
   <si>
     <t>INPUT PARAMETERS</t>
   </si>
@@ -101,24 +101,6 @@
     <t>Error</t>
   </si>
   <si>
-    <t>12k+360</t>
-  </si>
-  <si>
-    <t>6200+360</t>
-  </si>
-  <si>
-    <t>10k // 75k</t>
-  </si>
-  <si>
-    <t>8,2k // 110k</t>
-  </si>
-  <si>
-    <t>11k // 750k</t>
-  </si>
-  <si>
-    <t>6,2k // 300k</t>
-  </si>
-  <si>
     <t>1n</t>
   </si>
   <si>
@@ -126,6 +108,39 @@
   </si>
   <si>
     <t>6,2k // 150k</t>
+  </si>
+  <si>
+    <t>5100||33000</t>
+  </si>
+  <si>
+    <t>divisor</t>
+  </si>
+  <si>
+    <t>82k</t>
+  </si>
+  <si>
+    <t>91K||820K</t>
+  </si>
+  <si>
+    <t>4K7+680</t>
+  </si>
+  <si>
+    <t>24k+240</t>
+  </si>
+  <si>
+    <t>7k5||360k</t>
+  </si>
+  <si>
+    <t>20k||200k</t>
+  </si>
+  <si>
+    <t>13k||16k</t>
+  </si>
+  <si>
+    <t>9k1+270</t>
+  </si>
+  <si>
+    <t>30k||430K</t>
   </si>
 </sst>
 </file>
@@ -199,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +231,12 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,16 +313,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>99743</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>137402</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>572183</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>129782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -324,7 +345,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="144780" y="83820"/>
+          <a:off x="6164580" y="1173480"/>
           <a:ext cx="7879763" cy="2796782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -436,7 +457,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -731,36 +752,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC84E85-A155-4498-A788-00DEB25C7254}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCC4635-9E65-4A08-921F-1C13F6391E43}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" t="s">
         <v>16</v>
       </c>
@@ -803,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -818,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,11 +867,11 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
@@ -863,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -938,37 +973,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF2E8C6-91AD-447B-AF4A-DEB2930590A6}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" t="s">
         <v>16</v>
       </c>
@@ -1011,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1026,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1040,11 +1075,11 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
@@ -1071,7 +1106,20 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1084,6 +1132,12 @@
       <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F15">
+        <v>28022</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1115,215 +1169,6 @@
       <c r="D17" s="8">
         <f>ABS(B17-C17)/B17</f>
         <v>0.72290909090909106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <f>E8</f>
-        <v>10000</v>
-      </c>
-      <c r="C18">
-        <v>10000</v>
-      </c>
-      <c r="D18" s="8">
-        <f t="shared" ref="D18" si="0">ABS(B18-C18)/B18</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D7:F7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F93E34-39AF-488C-9A70-0E4A656E6C1E}">
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1.45</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6">
-        <f>2-(1/B3)</f>
-        <v>1.3103448275862069</v>
-      </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3">
-        <v>18029.39</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="7">
-        <f>1/(B4*E9*2*PI())</f>
-        <v>8827.5278915091058</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6">
-        <f>E8/E3</f>
-        <v>7631.5789473684217</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="6">
-        <f>1+E3</f>
-        <v>2.3103448275862069</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3">
-        <v>10000</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="9">
-        <f>E4</f>
-        <v>8827.5278915091058</v>
-      </c>
-      <c r="C16">
-        <f>1/((1/10000)+(1/75000))</f>
-        <v>8823.5294117647045</v>
-      </c>
-      <c r="D16" s="8">
-        <f>ABS(B16-C16)/B16</f>
-        <v>4.5295577578942175E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <f>E5</f>
-        <v>7631.5789473684217</v>
-      </c>
-      <c r="C17">
-        <f>1/((1/8200)+(1/110000))</f>
-        <v>7631.1336717428094</v>
-      </c>
-      <c r="D17" s="8">
-        <f>ABS(B17-C17)/B17</f>
-        <v>5.8346461287134114E-5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1355,36 +1200,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C32F953-FC33-4C44-82F1-C49EC063D04C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F93E34-39AF-488C-9A70-0E4A656E6C1E}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" t="s">
         <v>16</v>
       </c>
@@ -1394,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>2.82</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="5" t="s">
@@ -1402,7 +1247,7 @@
       </c>
       <c r="E3" s="6">
         <f>2-(1/B3)</f>
-        <v>1.6453900709219857</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -1411,7 +1256,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <v>14683.92</v>
+        <v>21646.44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1421,13 +1266,13 @@
       </c>
       <c r="E4" s="7">
         <f>1/(B4*E9*2*PI())</f>
-        <v>10838.723112894604</v>
+        <v>7352.4765777603779</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1436,13 +1281,13 @@
       </c>
       <c r="E5" s="6">
         <f>E8/E3</f>
-        <v>6077.5862068965516</v>
+        <v>10000</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1451,16 +1296,16 @@
       </c>
       <c r="E6" s="6">
         <f>1+E3</f>
-        <v>2.6453900709219855</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
@@ -1487,7 +1332,12 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1500,6 +1350,12 @@
       <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1507,15 +1363,21 @@
       </c>
       <c r="B16" s="9">
         <f>E4</f>
-        <v>10838.723112894604</v>
+        <v>7352.4765777603779</v>
       </c>
       <c r="C16">
-        <f>1/((1/11000)+(1/750000))</f>
-        <v>10840.998685939554</v>
+        <f>1/((1/10000)+(1/75000))</f>
+        <v>8823.5294117647045</v>
       </c>
       <c r="D16" s="8">
         <f>ABS(B16-C16)/B16</f>
-        <v>2.0994844330349664E-4</v>
+        <v>0.20007582730068632</v>
+      </c>
+      <c r="F16">
+        <v>18169</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1524,15 +1386,15 @@
       </c>
       <c r="B17">
         <f>E5</f>
-        <v>6077.5862068965516</v>
+        <v>10000</v>
       </c>
       <c r="C17">
-        <f>1/((1/6200)+(1/300000))</f>
-        <v>6074.4611365120836</v>
+        <f>1/((1/8200)+(1/110000))</f>
+        <v>7631.1336717428094</v>
       </c>
       <c r="D17" s="8">
         <f>ABS(B17-C17)/B17</f>
-        <v>5.1419597815360288E-4</v>
+        <v>0.23688663282571906</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1563,10 +1425,405 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C32F953-FC33-4C44-82F1-C49EC063D04C}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <f>2-(1/B3)</f>
+        <v>0.41269841269841279</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>29563.4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7">
+        <f>1/(B4*E9*2*PI())</f>
+        <v>5383.5128263966708</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6">
+        <f>E8/E3</f>
+        <v>24230.769230769227</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6">
+        <f>1+E3</f>
+        <v>1.4126984126984128</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="9">
+        <f>E4</f>
+        <v>5383.5128263966708</v>
+      </c>
+      <c r="C16">
+        <f>1/((1/11000)+(1/750000))</f>
+        <v>10840.998685939554</v>
+      </c>
+      <c r="D16" s="8">
+        <f>ABS(B16-C16)/B16</f>
+        <v>1.0137406625620924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>E5</f>
+        <v>24230.769230769227</v>
+      </c>
+      <c r="C17">
+        <f>1/((1/6200)+(1/300000))</f>
+        <v>6074.4611365120836</v>
+      </c>
+      <c r="D17" s="8">
+        <f>ABS(B17-C17)/B17</f>
+        <v>0.7493079530963267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <f>E8</f>
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>10000</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" ref="D18" si="0">ABS(B18-C18)/B18</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178F469F-B4E4-4A85-ADB0-2F9709EBF980}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <f>2-(1/B3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>36040</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7">
+        <f>1/(B4*E9*2*PI())</f>
+        <v>4416.0639037706806</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="e">
+        <f>E8/E3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6">
+        <f>1+E3</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1684,25 +1941,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD028AB-6018-4F69-99CF-ED77B61CB232}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA36C70-7BC2-4EDA-B68E-A8A7DF90E22A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1724,9 +1971,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA36C70-7BC2-4EDA-B68E-A8A7DF90E22A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD028AB-6018-4F69-99CF-ED77B61CB232}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>